<commit_message>
Product backlog/ users stories bewerkt
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a722794054318f2/Bureaublad/Ma/bewijzenmap/periode1.2/ADV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{2CD08D9C-3590-4458-A398-BBBDDAF93A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89A8BC4C-7D10-4894-B3A3-0F86A0458EEC}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{2CD08D9C-3590-4458-A398-BBBDDAF93A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D65987-FF31-435A-94E8-B2775835D0D6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1851505D-FFA6-43F4-AF70-416687379BC3}"/>
+    <workbookView xWindow="15645" yWindow="1770" windowWidth="21600" windowHeight="11505" xr2:uid="{1851505D-FFA6-43F4-AF70-416687379BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>een overzicht hebben over alle tentoonstellingen</t>
-  </si>
-  <si>
-    <t>weet wat kan verwachten</t>
   </si>
   <si>
     <t>een navigatie balk hebben</t>
@@ -212,15 +209,6 @@
     <t>weet of ik wel naar dit museum wil gaan</t>
   </si>
   <si>
-    <t>zodat ik mijn intresses kan vergroten</t>
-  </si>
-  <si>
-    <t>tentoonstellingen kunnen bekijken</t>
-  </si>
-  <si>
-    <t>weet wat ik kan zien in het museum</t>
-  </si>
-  <si>
     <t>een online tour kunnen zien</t>
   </si>
   <si>
@@ -240,6 +228,18 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>info voor scholen kunnen vinden</t>
+  </si>
+  <si>
+    <t>mischien een school reis naar het museum kan regelen</t>
+  </si>
+  <si>
+    <t>mijn intresses kan vergroten</t>
+  </si>
+  <si>
+    <t>weet wat ik kan verwachten</t>
   </si>
 </sst>
 </file>
@@ -661,22 +661,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294544DB-2322-448C-831B-3A7D69ECE91A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" customWidth="1"/>
-    <col min="4" max="4" width="45.21875" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" customWidth="1"/>
-    <col min="6" max="6" width="43" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -696,10 +696,10 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -713,27 +713,27 @@
         <v>8</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -744,173 +744,173 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>